<commit_message>
Move Fountain location based on world size.
</commit_message>
<xml_diff>
--- a/Part2/level31/fountainOfObjects/World Map.xlsx
+++ b/Part2/level31/fountainOfObjects/World Map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason\source\PlayersGuide\Part2\level31\fountainOfObjects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84403341-8F83-48DB-B1E6-6AD8868D5176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D6E8792-D7E7-4712-8744-90676EEC8735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1245" yWindow="195" windowWidth="26265" windowHeight="15210" xr2:uid="{6A7CC8C8-4FBE-4BE3-8BE2-003D72723DA9}"/>
   </bookViews>
@@ -225,13 +225,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -250,24 +247,24 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -588,7 +585,7 @@
   <dimension ref="A1:Z15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="28.35" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -597,354 +594,352 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="28.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="H1" s="10" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="H1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="Q1" s="10" t="s">
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="Q1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
     </row>
     <row r="2" spans="1:26" ht="28.35" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:26" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="6">
+      <c r="A3" s="8"/>
+      <c r="B3" s="5">
         <v>0</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>1</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>2</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>3</v>
       </c>
-      <c r="H3" s="13"/>
-      <c r="I3" s="4">
+      <c r="H3" s="9"/>
+      <c r="I3" s="3">
         <v>0</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="3">
         <v>1</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="3">
         <v>2</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L3" s="3">
         <v>3</v>
       </c>
-      <c r="M3" s="14">
+      <c r="M3" s="3">
         <v>4</v>
       </c>
-      <c r="N3" s="14">
+      <c r="N3" s="3">
         <v>5</v>
       </c>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="4">
+      <c r="Q3" s="9"/>
+      <c r="R3" s="3">
         <v>0</v>
       </c>
-      <c r="S3" s="4">
+      <c r="S3" s="3">
         <v>1</v>
       </c>
-      <c r="T3" s="4">
+      <c r="T3" s="3">
         <v>2</v>
       </c>
-      <c r="U3" s="4">
+      <c r="U3" s="3">
         <v>3</v>
       </c>
-      <c r="V3" s="4">
+      <c r="V3" s="3">
         <v>4</v>
       </c>
-      <c r="W3" s="4">
+      <c r="W3" s="3">
         <v>5</v>
       </c>
-      <c r="X3" s="4">
+      <c r="X3" s="3">
         <v>6</v>
       </c>
-      <c r="Y3" s="4">
+      <c r="Y3" s="3">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
+      <c r="A4" s="6">
         <v>0</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="11" t="s">
+      <c r="B4" s="7"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="3">
         <v>0</v>
       </c>
-      <c r="I4" s="15"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="11" t="s">
+      <c r="I4" s="10"/>
+      <c r="J4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Q4" s="4">
+      <c r="Q4" s="3">
         <v>0</v>
       </c>
-      <c r="S4" s="4"/>
-      <c r="T4" s="5"/>
-      <c r="U4" s="4"/>
-      <c r="V4" s="15"/>
-      <c r="W4" s="15"/>
-      <c r="X4" s="15"/>
-      <c r="Y4" s="15"/>
-      <c r="Z4" s="11" t="s">
+      <c r="S4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="10"/>
+      <c r="X4" s="10"/>
+      <c r="Y4" s="10"/>
+      <c r="Z4" s="15" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
+      <c r="A5" s="6">
         <v>1</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="11"/>
-      <c r="H5" s="4">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="15"/>
+      <c r="H5" s="3">
         <v>1</v>
       </c>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="11"/>
-      <c r="Q5" s="4">
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="15"/>
+      <c r="Q5" s="3">
         <v>1</v>
       </c>
-      <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
-      <c r="T5" s="4"/>
-      <c r="U5" s="4"/>
-      <c r="V5" s="15"/>
-      <c r="W5" s="15"/>
-      <c r="X5" s="15"/>
-      <c r="Y5" s="15"/>
-      <c r="Z5" s="11"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="10"/>
+      <c r="W5" s="10"/>
+      <c r="X5" s="10"/>
+      <c r="Y5" s="10"/>
+      <c r="Z5" s="15"/>
     </row>
     <row r="6" spans="1:26" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>2</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="11"/>
-      <c r="H6" s="4">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="15"/>
+      <c r="H6" s="3">
         <v>2</v>
       </c>
       <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="11"/>
-      <c r="Q6" s="4">
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="15"/>
+      <c r="Q6" s="3">
         <v>2</v>
       </c>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
-      <c r="T6" s="4"/>
-      <c r="U6" s="4"/>
-      <c r="V6" s="15"/>
-      <c r="W6" s="15"/>
-      <c r="X6" s="15"/>
-      <c r="Y6" s="16"/>
-      <c r="Z6" s="11"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="10"/>
+      <c r="W6" s="10"/>
+      <c r="X6" s="10"/>
+      <c r="Y6" s="11"/>
+      <c r="Z6" s="15"/>
     </row>
     <row r="7" spans="1:26" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>3</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="11"/>
-      <c r="H7" s="4">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="15"/>
+      <c r="H7" s="3">
         <v>3</v>
       </c>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="11"/>
-      <c r="Q7" s="4">
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="15"/>
+      <c r="Q7" s="3">
         <v>3</v>
       </c>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
-      <c r="T7" s="4"/>
-      <c r="U7" s="4"/>
-      <c r="V7" s="15"/>
-      <c r="W7" s="15"/>
-      <c r="X7" s="15"/>
-      <c r="Y7" s="15"/>
-      <c r="Z7" s="11"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="10"/>
+      <c r="W7" s="10"/>
+      <c r="X7" s="10"/>
+      <c r="Y7" s="10"/>
+      <c r="Z7" s="15"/>
     </row>
     <row r="8" spans="1:26" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="H8" s="14">
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="H8" s="3">
         <v>4</v>
       </c>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="11"/>
-      <c r="Q8" s="4">
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="15"/>
+      <c r="Q8" s="3">
         <v>4</v>
       </c>
-      <c r="R8" s="15"/>
-      <c r="S8" s="15"/>
-      <c r="T8" s="15"/>
-      <c r="U8" s="15"/>
-      <c r="V8" s="15"/>
-      <c r="W8" s="15"/>
-      <c r="X8" s="15"/>
-      <c r="Y8" s="15"/>
-      <c r="Z8" s="11"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="10"/>
+      <c r="W8" s="10"/>
+      <c r="X8" s="10"/>
+      <c r="Y8" s="10"/>
+      <c r="Z8" s="15"/>
     </row>
     <row r="9" spans="1:26" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H9" s="14">
+      <c r="H9" s="3">
         <v>5</v>
       </c>
-      <c r="I9" s="15"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="11"/>
-      <c r="Q9" s="4">
+      <c r="I9" s="10"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="15"/>
+      <c r="Q9" s="3">
         <v>5</v>
       </c>
-      <c r="R9" s="15"/>
-      <c r="S9" s="15"/>
-      <c r="T9" s="15"/>
-      <c r="U9" s="15"/>
-      <c r="V9" s="15"/>
-      <c r="W9" s="15"/>
-      <c r="X9" s="15"/>
-      <c r="Y9" s="15"/>
-      <c r="Z9" s="11"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="12"/>
+      <c r="U9" s="10"/>
+      <c r="V9" s="10"/>
+      <c r="W9" s="10"/>
+      <c r="X9" s="10"/>
+      <c r="Y9" s="10"/>
+      <c r="Z9" s="15"/>
     </row>
     <row r="10" spans="1:26" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I10" s="12" t="s">
+      <c r="I10" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="Q10" s="4">
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="Q10" s="3">
         <v>6</v>
       </c>
-      <c r="R10" s="15"/>
-      <c r="S10" s="15"/>
-      <c r="T10" s="15"/>
-      <c r="U10" s="15"/>
-      <c r="V10" s="15"/>
-      <c r="W10" s="15"/>
-      <c r="X10" s="15"/>
-      <c r="Y10" s="15"/>
-      <c r="Z10" s="11"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="10"/>
+      <c r="W10" s="10"/>
+      <c r="X10" s="10"/>
+      <c r="Y10" s="10"/>
+      <c r="Z10" s="15"/>
     </row>
     <row r="11" spans="1:26" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="Q11" s="4">
+      <c r="Q11" s="3">
         <v>7</v>
       </c>
-      <c r="R11" s="15"/>
-      <c r="S11" s="15"/>
-      <c r="T11" s="15"/>
-      <c r="U11" s="15"/>
-      <c r="V11" s="15"/>
-      <c r="W11" s="15"/>
-      <c r="X11" s="15"/>
-      <c r="Y11" s="15"/>
-      <c r="Z11" s="11"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="10"/>
+      <c r="V11" s="10"/>
+      <c r="W11" s="10"/>
+      <c r="X11" s="10"/>
+      <c r="Y11" s="10"/>
+      <c r="Z11" s="15"/>
     </row>
     <row r="12" spans="1:26" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="R12" s="12" t="s">
+      <c r="R12" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="S12" s="12"/>
-      <c r="T12" s="12"/>
-      <c r="U12" s="12"/>
-      <c r="V12" s="12"/>
-      <c r="W12" s="12"/>
-      <c r="X12" s="12"/>
-      <c r="Y12" s="12"/>
+      <c r="S12" s="16"/>
+      <c r="T12" s="16"/>
+      <c r="U12" s="16"/>
+      <c r="V12" s="16"/>
+      <c r="W12" s="16"/>
+      <c r="X12" s="16"/>
+      <c r="Y12" s="16"/>
     </row>
     <row r="14" spans="1:26" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L14" s="1"/>
-      <c r="M14" s="3" t="s">
+      <c r="M14" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
     </row>
     <row r="15" spans="1:26" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L15" s="2"/>
-      <c r="M15" s="3" t="s">
+      <c r="M15" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="M15:P15"/>
-    <mergeCell ref="Q1:U1"/>
-    <mergeCell ref="Z4:Z11"/>
-    <mergeCell ref="R12:Y12"/>
-    <mergeCell ref="M14:P14"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="H1:L1"/>
     <mergeCell ref="O4:O9"/>
     <mergeCell ref="I10:N10"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="F4:F7"/>
+    <mergeCell ref="M15:P15"/>
+    <mergeCell ref="Q1:U1"/>
+    <mergeCell ref="Z4:Z11"/>
+    <mergeCell ref="R12:Y12"/>
+    <mergeCell ref="M14:P14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>